<commit_message>
Update test cases and requirement
Thêm test cases and đưa lên file Xác định yêu cầu
</commit_message>
<xml_diff>
--- a/BaiTapLon_TestCases.xlsx
+++ b/BaiTapLon_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kiem Thu Phan Mem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D207DD1-AB40-48DC-B8C0-6129B8C558D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF8AB56-2448-4E0D-B696-5A41281E55F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{12BF696D-D391-48CC-93C0-8956F0C07BCD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>Test Cases ID</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>TC-001</t>
@@ -327,6 +324,401 @@
   </si>
   <si>
     <t>Sign Up Form - Đăng Ký</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create new account successfully</t>
+  </si>
+  <si>
+    <r>
+      <t>1. Launch application.
+2. Click on '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Đăng Ký</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' button.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. On '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Đăng Ký</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' form, input username on '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tên tài khoản</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' field.
+2. Input password on '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Password</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' field.
+3.  Input Last Name on '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Họ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' field.
+4.  Input First Name on '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tên</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' field.
+5. Input email address on '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' field.
+6. Select a value on '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Loại tài khoản</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' dropdown.
+7. Click on '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Đăng ký</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' button.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7. Alert dialog is displayed with below components:
+- Message: "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Thêm thành công!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"
+- Description: "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Thêm User thành công</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button</t>
+    </r>
+  </si>
+  <si>
+    <t>Username: hieuuser
+Password: 12345
+Họ: Trần.
+Tên: Hiếu.
+Email: hieu@gmail.com
+Loại tài khoản: user</t>
+  </si>
+  <si>
+    <t>TC-005</t>
+  </si>
+  <si>
+    <t>Verify that user is NOT able to create new account with exsited username</t>
+  </si>
+  <si>
+    <t>TC-006</t>
+  </si>
+  <si>
+    <t>Home - Trang Chủ</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Student user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is NOT able to view </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Edit menu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>**Create a user with '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Loại tài khoản</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">' = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Student)</t>
+    </r>
+  </si>
+  <si>
+    <t>4. On Home page, the Edit menu is NOT visible for this Student user</t>
+  </si>
+  <si>
+    <t>Username: hieustudent
+Password: 12345
+Họ: Trần.
+Tên: Hiếu.
+Email: hieustudent@gmail.com
+Loại tài khoản: Student</t>
   </si>
 </sst>
 </file>
@@ -391,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -401,19 +793,35 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -425,6 +833,41 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -738,21 +1181,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E047EEFD-2B50-4D13-AAE0-2DE4002BFB4E}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.21875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
     <col min="5" max="5" width="35.44140625" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.77734375" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
     <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -763,7 +1206,7 @@
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -784,103 +1227,185 @@
     </row>
     <row r="2" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="C3" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="F7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>9</v>
-      </c>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C8"/>
+      <c r="D8" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H5">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",H2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",H2)))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",H6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",H6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",H7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",H7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H5" xr:uid="{F24804AC-4EC7-4A07-968B-ED199A49B7EC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H7" xr:uid="{F24804AC-4EC7-4A07-968B-ED199A49B7EC}">
       <formula1>"Pass, Fail, Block, N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>